<commit_message>
Correct tables after realizing outputs were off from running only one section of the script
</commit_message>
<xml_diff>
--- a/submission/table_S14_combined_top20_otus_each_model.xlsx
+++ b/submission/table_S14_combined_top20_otus_each_model.xlsx
@@ -349,7 +349,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>family</t>
+          <t>OTU</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -371,14 +371,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Clostridiaceae 1</t>
+          <t>Desulfovibrio (OTU 3465)</t>
         </is>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="C2">
-        <v>0.481322659237805</v>
+        <v>-0.3296925030340111</v>
       </c>
       <c r="D2">
         <v>-1</v>
@@ -387,14 +387,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sutterellaceae</t>
+          <t>Ruminococcaceae (OTU 467)</t>
         </is>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="C3">
-        <v>-0.4740904078638372</v>
+        <v>0.4074428019338807</v>
       </c>
       <c r="D3">
         <v>-1</v>
@@ -403,14 +403,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Clostridia Unclassified</t>
+          <t>Lachnospiraceae (OTU 543)</t>
         </is>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>-0.4506934929230019</v>
+        <v>-0.3400803900547354</v>
       </c>
       <c r="D4">
         <v>-1</v>
@@ -419,14 +419,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Deferribacteraceae</t>
+          <t>Erysipelotrichaceae (OTU 189)</t>
         </is>
       </c>
       <c r="B5">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>-0.3994487262081577</v>
+        <v>0.3535074191234203</v>
       </c>
       <c r="D5">
         <v>-1</v>
@@ -435,14 +435,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Burkholderiales Unclassified</t>
+          <t>Porphyromonadaceae (OTU 228)</t>
         </is>
       </c>
       <c r="B6">
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
       <c r="C6">
-        <v>-0.4016562852281997</v>
+        <v>0.3180013784902163</v>
       </c>
       <c r="D6">
         <v>-1</v>
@@ -451,14 +451,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Rikenellaceae</t>
+          <t>Betaproteobacteria (OTU 58)</t>
         </is>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>0.3408740360041195</v>
+        <v>-0.1839360244793108</v>
       </c>
       <c r="D7">
         <v>-1</v>
@@ -467,14 +467,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Staphylococcaceae</t>
+          <t>Enterobacteriaceae (OTU 1)</t>
         </is>
       </c>
       <c r="B8">
-        <v>13.5</v>
+        <v>14.5</v>
       </c>
       <c r="C8">
-        <v>-0.3702919271248298</v>
+        <v>-0.1838742192593545</v>
       </c>
       <c r="D8">
         <v>-1</v>
@@ -483,14 +483,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Desulfovibrionales Unclassified</t>
+          <t>Enterococcus (OTU 23)</t>
         </is>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0.05785592268785095</v>
+        <v>-0.1692471862407768</v>
       </c>
       <c r="D9">
         <v>-1</v>
@@ -499,14 +499,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Flavobacteriaceae</t>
+          <t>Porphyromonadaceae (OTU 139)</t>
         </is>
       </c>
       <c r="B10">
-        <v>16.5</v>
+        <v>19.5</v>
       </c>
       <c r="C10">
-        <v>-0.1925389041120648</v>
+        <v>0.2965338002606991</v>
       </c>
       <c r="D10">
         <v>-1</v>
@@ -515,14 +515,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Proteobacteria Unclassified</t>
+          <t>Lachnospiraceae (OTU 397)</t>
         </is>
       </c>
       <c r="B11">
-        <v>18</v>
+        <v>19.5</v>
       </c>
       <c r="C11">
-        <v>0.1866353477695882</v>
+        <v>-0.2597015998577158</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -531,14 +531,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Peptostreptococcaceae</t>
+          <t>Burkholderiales (OTU 34)</t>
         </is>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>0.3011861827546056</v>
+        <v>-0.1733591678659266</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -547,14 +547,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ruminococcaceae</t>
+          <t>Porphyromonadaceae (OTU 87)</t>
         </is>
       </c>
       <c r="B13">
-        <v>19</v>
+        <v>23.5</v>
       </c>
       <c r="C13">
-        <v>0.2460960140035185</v>
+        <v>0.2699772801286908</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -563,14 +563,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cytophagaceae</t>
+          <t>Clostridium (OTU 154)</t>
         </is>
       </c>
       <c r="B14">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C14">
-        <v>-0.2640829755265243</v>
+        <v>-0.1562934472421492</v>
       </c>
       <c r="D14">
         <v>-1</v>
@@ -579,14 +579,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bacteroidaceae</t>
+          <t>Porphyromonadaceae (OTU 608)</t>
         </is>
       </c>
       <c r="B15">
-        <v>19.5</v>
+        <v>26</v>
       </c>
       <c r="C15">
-        <v>-0.2800504736700357</v>
+        <v>0.2711412609900756</v>
       </c>
       <c r="D15">
         <v>-1</v>
@@ -595,14 +595,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Coriobacteriaceae</t>
+          <t>Porphyromonadaceae (OTU 222)</t>
         </is>
       </c>
       <c r="B16">
-        <v>19.5</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>0.2950627103946124</v>
+        <v>0.253072086268029</v>
       </c>
       <c r="D16">
         <v>-1</v>
@@ -611,14 +611,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Streptococcaceae</t>
+          <t>Ruminococcaceae (OTU 520)</t>
         </is>
       </c>
       <c r="B17">
-        <v>20.5</v>
+        <v>30.5</v>
       </c>
       <c r="C17">
-        <v>-0.2562655957946502</v>
+        <v>-0.1553644695555795</v>
       </c>
       <c r="D17">
         <v>-1</v>
@@ -627,14 +627,14 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Rhodospirillaceae</t>
+          <t>Bacillus (OTU 636)</t>
         </is>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>31.5</v>
       </c>
       <c r="C18">
-        <v>-0.2545390919992014</v>
+        <v>-0.1553644695555795</v>
       </c>
       <c r="D18">
         <v>-1</v>
@@ -643,14 +643,14 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Gp2 Unclassified</t>
+          <t>Dactylosporangium (OTU 3207)</t>
         </is>
       </c>
       <c r="B19">
-        <v>21.5</v>
+        <v>32.5</v>
       </c>
       <c r="C19">
-        <v>-0.2562655957946502</v>
+        <v>-0.1553644695555795</v>
       </c>
       <c r="D19">
         <v>-1</v>
@@ -659,14 +659,14 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Clostridiales Incertae Sedis XIII</t>
+          <t>Coriobacteriaceae (OTU 293)</t>
         </is>
       </c>
       <c r="B20">
-        <v>22</v>
+        <v>34.5</v>
       </c>
       <c r="C20">
-        <v>0.02599038720686881</v>
+        <v>0.2492104073905196</v>
       </c>
       <c r="D20">
         <v>-1</v>
@@ -675,14 +675,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Veillonellaceae</t>
+          <t>Clostridiales (OTU 356)</t>
         </is>
       </c>
       <c r="B21">
-        <v>22.5</v>
+        <v>36.5</v>
       </c>
       <c r="C21">
-        <v>-0.1685523992131303</v>
+        <v>-0.243039217851724</v>
       </c>
       <c r="D21">
         <v>-1</v>
@@ -691,14 +691,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bacteroidaceae</t>
+          <t>Enterobacteriaceae (OTU 1)</t>
         </is>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>-0.5007118364051619</v>
+        <v>0.4805050429743277</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -707,14 +707,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ruminococcaceae</t>
+          <t>Bacteroides (OTU 2)</t>
         </is>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23">
-        <v>0.341988710051604</v>
+        <v>-0.452390011750085</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -723,14 +723,14 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Lactobacillales Unclassified</t>
+          <t>Lactobacillus (OTU 18)</t>
         </is>
       </c>
       <c r="B24">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>0.3188234693598958</v>
+        <v>-0.4092711501860915</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -739,14 +739,14 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Deferribacteraceae</t>
+          <t>Escherichia/Shigella (OTU 610)</t>
         </is>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="C25">
-        <v>-0.3284570316690428</v>
+        <v>-0.3211501162625571</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -755,14 +755,14 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Staphylococcaceae</t>
+          <t>Lachnospiraceae (OTU 56)</t>
         </is>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>-0.2933488391099328</v>
+        <v>0.2834676535132536</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -771,14 +771,14 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Enterobacteriaceae</t>
+          <t>Ruminococcaceae (OTU 520)</t>
         </is>
       </c>
       <c r="B27">
-        <v>10</v>
+        <v>13.5</v>
       </c>
       <c r="C27">
-        <v>0.2284122427956992</v>
+        <v>-0.287966761885177</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -787,14 +787,14 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Bifidobacteriaceae</t>
+          <t>Porphyromonadaceae (OTU 54)</t>
         </is>
       </c>
       <c r="B28">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>0.1939747560030551</v>
+        <v>-0.2011592266132916</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -803,14 +803,14 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Unclassified</t>
+          <t>Porphyromonadaceae (OTU 22)</t>
         </is>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>-0.07914472247929742</v>
+        <v>0.2237962690648616</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -819,14 +819,14 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Bacilli Unclassified</t>
+          <t>Lachnospiraceae (OTU 38)</t>
         </is>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>-0.2012761607471513</v>
+        <v>-0.08215621458561985</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -835,14 +835,14 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Alteromonadaceae</t>
+          <t>Lachnospiraceae (OTU 33)</t>
         </is>
       </c>
       <c r="B31">
-        <v>14.5</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>-0.249347660923028</v>
+        <v>-0.2524117226522107</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -851,14 +851,14 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Enterococcaceae</t>
+          <t>Porphyromonadaceae (OTU 7)</t>
         </is>
       </c>
       <c r="B32">
-        <v>16.5</v>
+        <v>20</v>
       </c>
       <c r="C32">
-        <v>-0.1778472996908328</v>
+        <v>0.1314449678811958</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -867,14 +867,14 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Verrucomicrobiaceae</t>
+          <t>Ruminococcaceae (OTU 60)</t>
         </is>
       </c>
       <c r="B33">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C33">
-        <v>0.2399610204591707</v>
+        <v>-0.1139403081751913</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -883,14 +883,14 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Clostridiales Unclassified</t>
+          <t>Erysipelotrichaceae (OTU 234)</t>
         </is>
       </c>
       <c r="B34">
-        <v>18</v>
+        <v>24.5</v>
       </c>
       <c r="C34">
-        <v>0.1108810343206971</v>
+        <v>0.1968104657738282</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -899,14 +899,14 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Anaeroplasmataceae</t>
+          <t>Lachnospiraceae (OTU 9)</t>
         </is>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C35">
-        <v>0.0805697506873721</v>
+        <v>-0.2105210354545368</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -915,14 +915,14 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Fusobacteriaceae</t>
+          <t>Proteus (OTU 16)</t>
         </is>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C36">
-        <v>0.105184750449221</v>
+        <v>-0.190954390712031</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -931,14 +931,14 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Corynebacteriaceae</t>
+          <t>Alishewanella (OTU 776)</t>
         </is>
       </c>
       <c r="B37">
-        <v>18.5</v>
+        <v>27</v>
       </c>
       <c r="C37">
-        <v>0.04698624744230111</v>
+        <v>-0.1122260698812191</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -947,14 +947,14 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Coriobacteriaceae</t>
+          <t>Eisenbergiella (OTU 164)</t>
         </is>
       </c>
       <c r="B38">
-        <v>19</v>
+        <v>32.5</v>
       </c>
       <c r="C38">
-        <v>0.1838561888447812</v>
+        <v>-0.0456374695110339</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -963,14 +963,14 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Sphingobacteriaceae</t>
+          <t>Clostridium (OTU 99)</t>
         </is>
       </c>
       <c r="B39">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C39">
-        <v>-0.116475614095238</v>
+        <v>0.1805555754102407</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -979,14 +979,14 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Lachnospiraceae</t>
+          <t>Clostridium (OTU 226)</t>
         </is>
       </c>
       <c r="B40">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C40">
-        <v>0.1048601131973099</v>
+        <v>0.04605844444543253</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -995,14 +995,14 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Firmicutes Unclassified</t>
+          <t>Lactobacillus (OTU 834)</t>
         </is>
       </c>
       <c r="B41">
-        <v>20</v>
+        <v>33.5</v>
       </c>
       <c r="C41">
-        <v>-0.1388768458416531</v>
+        <v>-0.0456374695110339</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1011,14 +1011,14 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Bifidobacteriaceae</t>
+          <t>Lactobacillus (OTU 18)</t>
         </is>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42">
-        <v>2.025902829660961</v>
+        <v>-1.209561846396649</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -1027,14 +1027,14 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Enterococcaceae</t>
+          <t>Bacteroides (OTU 2)</t>
         </is>
       </c>
       <c r="B43">
         <v>4</v>
       </c>
       <c r="C43">
-        <v>-1.494202514784093</v>
+        <v>-1.044768312738835</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -1043,14 +1043,14 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Peptostreptococcaceae</t>
+          <t>Lachnospiraceae (OTU 35)</t>
         </is>
       </c>
       <c r="B44">
         <v>7</v>
       </c>
       <c r="C44">
-        <v>0.8394070445800451</v>
+        <v>0.8395257141727522</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -1059,14 +1059,14 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Desulfovibrionaceae</t>
+          <t>Coriobacteriaceae (OTU 3419)</t>
         </is>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>1.013900647953319</v>
+        <v>-0.4249008232572614</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -1075,14 +1075,14 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Lactobacillales Unclassified</t>
+          <t>Coriobacteriaceae (OTU 379)</t>
         </is>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>10.5</v>
       </c>
       <c r="C46">
-        <v>1.494277533622491</v>
+        <v>0.8030734725326898</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1091,14 +1091,14 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Erysipelotrichaceae</t>
+          <t>Turicibacter (OTU 14)</t>
         </is>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>11.5</v>
       </c>
       <c r="C47">
-        <v>1.178557978718739</v>
+        <v>0.6296225168141147</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -1107,14 +1107,14 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Bacteroidaceae</t>
+          <t>Bifidobacterium (OTU 46)</t>
         </is>
       </c>
       <c r="B48">
         <v>12</v>
       </c>
       <c r="C48">
-        <v>-1.04785378972747</v>
+        <v>0.7453827213448163</v>
       </c>
       <c r="D48">
         <v>1</v>
@@ -1123,14 +1123,14 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Eubacteriaceae</t>
+          <t>Bacteroides (OTU 3)</t>
         </is>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="C49">
-        <v>-0.9293192854326615</v>
+        <v>0.6747382360394445</v>
       </c>
       <c r="D49">
         <v>1</v>
@@ -1139,14 +1139,14 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Verrucomicrobiaceae</t>
+          <t>Enterococcus (OTU 23)</t>
         </is>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="C50">
-        <v>0.6730869650730957</v>
+        <v>-0.6034903369986337</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1155,14 +1155,14 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Ruminococcaceae</t>
+          <t>Porphyromonadaceae (OTU 7)</t>
         </is>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>17.5</v>
       </c>
       <c r="C51">
-        <v>-0.9383543019083237</v>
+        <v>0.6152684912951247</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -1171,14 +1171,14 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Deltaproteobacteria Unclassified</t>
+          <t>Erysipelotrichaceae (OTU 234)</t>
         </is>
       </c>
       <c r="B52">
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
       <c r="C52">
-        <v>0.9654870966319133</v>
+        <v>0.6021268407672054</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -1187,14 +1187,14 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Prevotellaceae</t>
+          <t>Bacteria (OTU 509)</t>
         </is>
       </c>
       <c r="B53">
-        <v>18.5</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>-0.6982273878146765</v>
+        <v>0.6066825319705877</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -1203,14 +1203,14 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Clostridiaceae 1</t>
+          <t>Lachnospiraceae (OTU 44)</t>
         </is>
       </c>
       <c r="B54">
-        <v>19.5</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>-0.6850383402094689</v>
+        <v>0.5807993220192496</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -1219,14 +1219,14 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Proteobacteria Unclassified</t>
+          <t>Lactobacillus (OTU 31)</t>
         </is>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C55">
-        <v>-0.4831945124862168</v>
+        <v>0.5531318973366881</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -1235,14 +1235,14 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Pseudomonadaceae</t>
+          <t>Lactobacillales (OTU 603)</t>
         </is>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C56">
-        <v>-0.6389767874501737</v>
+        <v>0.5721851142342991</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -1251,14 +1251,14 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Actinomycetales Unclassified</t>
+          <t>Bacteroides (OTU 32)</t>
         </is>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C57">
-        <v>-0.6982273878146765</v>
+        <v>0.1162382837427073</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -1267,14 +1267,14 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Coriobacteriaceae</t>
+          <t>Alistipes (OTU 161)</t>
         </is>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C58">
-        <v>0.5549978617799494</v>
+        <v>0.09003603176770333</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1283,14 +1283,14 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Burkholderiaceae</t>
+          <t>Anaerofustis (OTU 475)</t>
         </is>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C59">
-        <v>-0.06691665097576682</v>
+        <v>-0.4718461291268826</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -1299,14 +1299,14 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Lachnospiraceae</t>
+          <t>Lachnospiraceae (OTU 109)</t>
         </is>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>28.5</v>
       </c>
       <c r="C60">
-        <v>0.527694606514816</v>
+        <v>0.009322759602494523</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1315,14 +1315,14 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Bacillales Unclassified</t>
+          <t>Streptococcus (OTU 512)</t>
         </is>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>28.5</v>
       </c>
       <c r="C61">
-        <v>-0.06691665097576682</v>
+        <v>0.530449090825015</v>
       </c>
       <c r="D61">
         <v>1</v>

</xml_diff>